<commit_message>
Added a few more responses
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\issac\OneDrive\Desktop\Documents\UM\2020 2021 Semester 2\WID3002 NATURAL LANGUAGE PROCESSING\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven\Documents\GitHub\NLP-bank-chatbot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC05E3E4-60C5-4CA1-A237-53BA2A6A5A58}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA193E7C-6144-4718-9F24-3DF0BEFDCB1C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GENERAL_INTENTS" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>It is free of charge.</t>
   </si>
@@ -115,6 +115,24 @@
   </si>
   <si>
     <t>answer</t>
+  </si>
+  <si>
+    <t>Hi</t>
+  </si>
+  <si>
+    <t>Hello, how may I help you?</t>
+  </si>
+  <si>
+    <t>Bye</t>
+  </si>
+  <si>
+    <t>Goodbye, have a nice day.</t>
+  </si>
+  <si>
+    <t>I want to deposit AMOUNT</t>
+  </si>
+  <si>
+    <t>AMOUNT has been deposited into</t>
   </si>
 </sst>
 </file>
@@ -142,7 +160,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -165,11 +183,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -178,6 +207,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,19 +425,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB0B082F-789D-46DC-A03C-2A4A6841A2A1}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="51.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -413,7 +445,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -421,7 +453,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -429,12 +461,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>27</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -448,19 +488,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="53.109375" customWidth="1"/>
-    <col min="2" max="2" width="101.6640625" customWidth="1"/>
+    <col min="1" max="1" width="53.140625" customWidth="1"/>
+    <col min="2" max="2" width="101.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -468,7 +508,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -476,7 +516,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -484,7 +524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -492,7 +532,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -500,7 +540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -508,7 +548,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -516,7 +556,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -524,7 +564,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -532,7 +572,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -540,12 +580,28 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -562,13 +618,13 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.33203125" customWidth="1"/>
-    <col min="2" max="2" width="44.109375" customWidth="1"/>
+    <col min="1" max="1" width="31.28515625" customWidth="1"/>
+    <col min="2" max="2" width="44.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -576,7 +632,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>24</v>
       </c>
@@ -584,11 +640,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
     </row>

</xml_diff>

<commit_message>
Added a few more FAQ
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven\Documents\GitHub\NLP-bank-chatbot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goy\Documents\GitHub\NLP-bank-chatbot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA193E7C-6144-4718-9F24-3DF0BEFDCB1C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EDA3C33-5FDC-478E-90B0-4666AAC7A9C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GENERAL_INTENTS" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
   <si>
     <t>It is free of charge.</t>
   </si>
@@ -133,13 +133,53 @@
   </si>
   <si>
     <t>AMOUNT has been deposited into</t>
+  </si>
+  <si>
+    <t>Connect me to an agent</t>
+  </si>
+  <si>
+    <t>Why do I need a TAC?</t>
+  </si>
+  <si>
+    <t>TAC is compulsory for specific transactions because it provides an additional layer of security to protect you against unauthorised access to your account.</t>
+  </si>
+  <si>
+    <t>Is TAC the same as the Internet Banking PIN?</t>
+  </si>
+  <si>
+    <t>No, it's different. Your Internet Banking PIN, which is issued at the Branch, allows you to register for Maybank2u.com. The TAC is not used for login but only for specific transactions and types of activities.</t>
+  </si>
+  <si>
+    <t>How much time do I have before my TAC expires?</t>
+  </si>
+  <si>
+    <t>For your online banking safety, your TAC can now only be used while you are still logged on to Maybank2u.com. Your TAC will expire immediately each time you logout.</t>
+  </si>
+  <si>
+    <t>Do I need a TAC for every transaction?</t>
+  </si>
+  <si>
+    <t>Yes because you can only use one (1) TAC for only one (1) transaction or request.</t>
+  </si>
+  <si>
+    <t>What is the maximum transaction limit for 3rd Party Fund transfers, Interbank GIRO and Foreign Telegraphic Transfer?</t>
+  </si>
+  <si>
+    <t>Will my electronic statement be accepted in case of any dispute?</t>
+  </si>
+  <si>
+    <t>It is a valid document. All you have to do is obtain an endorsed copy at any Maybank branch in case of dispute or for other purposes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The maximum limit is RM50,000.
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -148,6 +188,11 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -198,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -208,6 +253,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -427,17 +479,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB0B082F-789D-46DC-A03C-2A4A6841A2A1}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -445,7 +497,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -453,7 +505,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -461,7 +513,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -469,7 +521,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -488,19 +540,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.140625" customWidth="1"/>
-    <col min="2" max="2" width="101.7109375" customWidth="1"/>
+    <col min="1" max="1" width="53.109375" customWidth="1"/>
+    <col min="2" max="2" width="126.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -508,7 +560,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -516,7 +568,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -524,7 +576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -532,7 +584,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -540,7 +592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -548,7 +600,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -556,7 +608,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="53.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -564,7 +616,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -572,7 +624,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -580,7 +632,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -588,7 +640,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>30</v>
       </c>
@@ -596,12 +648,68 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -618,13 +726,13 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.28515625" customWidth="1"/>
-    <col min="2" max="2" width="44.140625" customWidth="1"/>
+    <col min="1" max="1" width="31.33203125" customWidth="1"/>
+    <col min="2" max="2" width="44.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -632,7 +740,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>24</v>
       </c>
@@ -640,11 +748,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
     </row>

</xml_diff>

<commit_message>
Added BANK_BALANCE database and Improve on General Intent
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goy\Documents\GitHub\NLP-bank-chatbot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BrandonTan\Desktop\NLP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A40A972-C2AF-43B9-8FE5-D48D1144D40C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{675D3070-B963-4944-B68C-5F174F05F62D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GENERAL_INTENTS" sheetId="2" r:id="rId1"/>
     <sheet name="FAQS" sheetId="1" r:id="rId2"/>
     <sheet name="DEFAULT_REPLY" sheetId="3" r:id="rId3"/>
+    <sheet name="BANK_BALANCE" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
   <si>
     <t>It is free of charge.</t>
   </si>
@@ -44,12 +45,6 @@
     <t>Not all payee corporations process payments daily. Therefore, to avoid late payment, it's best to make your payments in advance. Please note that payments made after 12a.m. will only be credited the next working day.</t>
   </si>
   <si>
-    <t>Can I know the total balance in my bank account BANK_ACC</t>
-  </si>
-  <si>
-    <t>Your bank account BANK_ACC has a total balance of AMOUNT</t>
-  </si>
-  <si>
     <t>AMOUNT bill has been paid.</t>
   </si>
   <si>
@@ -105,9 +100,6 @@
     <t>I want to transfer AMOUNT to PERSON in BANK_ACC</t>
   </si>
   <si>
-    <t>AMOUNT has been transferred to PERSON in BANK_ACC</t>
-  </si>
-  <si>
     <t>I want to pay bill of AMOUNT with PERSON in BANK_ACC</t>
   </si>
   <si>
@@ -127,12 +119,6 @@
   </si>
   <si>
     <t>Goodbye, have a nice day.</t>
-  </si>
-  <si>
-    <t>I want to deposit AMOUNT</t>
-  </si>
-  <si>
-    <t>AMOUNT has been deposited into</t>
   </si>
   <si>
     <t>Connect me to an agent</t>
@@ -191,6 +177,27 @@
   </si>
   <si>
     <t>There is no expiry to your account. However, your account will be automatically deactivated if you do not login to within 6-12 months.</t>
+  </si>
+  <si>
+    <t>I want to deposit AMOUNT to BANK_ACC</t>
+  </si>
+  <si>
+    <t>AMOUNT has been deposited into BANK_ACC.</t>
+  </si>
+  <si>
+    <t>AMOUNT has been transferred to PERSON in BANK_ACC.</t>
+  </si>
+  <si>
+    <t>bank acc</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>BANK_ACC has AMOUNT left.</t>
+  </si>
+  <si>
+    <t>I want to check balance in BANK_ACC.</t>
   </si>
 </sst>
 </file>
@@ -495,57 +502,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB0B082F-789D-46DC-A03C-2A4A6841A2A1}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="51.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="53.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" t="s">
-        <v>35</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -560,7 +573,7 @@
   </sheetPr>
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A18" sqref="A18:B23"/>
     </sheetView>
   </sheetViews>
@@ -572,23 +585,23 @@
   <sheetData>
     <row r="1" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
@@ -596,15 +609,15 @@
     </row>
     <row r="4" spans="1:2" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>1</v>
@@ -612,15 +625,15 @@
     </row>
     <row r="6" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>2</v>
@@ -628,7 +641,7 @@
     </row>
     <row r="8" spans="1:2" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>3</v>
@@ -636,7 +649,7 @@
     </row>
     <row r="9" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>4</v>
@@ -644,15 +657,15 @@
     </row>
     <row r="10" spans="1:2" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>5</v>
@@ -660,23 +673,23 @@
     </row>
     <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>2</v>
@@ -684,74 +697,74 @@
     </row>
     <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -776,18 +789,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -802,4 +815,47 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE602675-32E7-41BB-B088-0029ED80F667}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>123456789</v>
+      </c>
+      <c r="B2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>987654321</v>
+      </c>
+      <c r="B3">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added approshpe for the bank acc
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BrandonTan\Desktop\NLP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{675D3070-B963-4944-B68C-5F174F05F62D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B463A4-0123-438D-BC35-C9F0EC0055C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GENERAL_INTENTS" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="59">
   <si>
     <t>It is free of charge.</t>
   </si>
@@ -198,6 +198,12 @@
   </si>
   <si>
     <t>I want to check balance in BANK_ACC.</t>
+  </si>
+  <si>
+    <t>123456789</t>
+  </si>
+  <si>
+    <t>987654321</t>
   </si>
 </sst>
 </file>
@@ -268,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -287,6 +293,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,7 +511,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB0B082F-789D-46DC-A03C-2A4A6841A2A1}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -821,8 +828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE602675-32E7-41BB-B088-0029ED80F667}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -839,16 +846,16 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>123456789</v>
+      <c r="A2" s="8" t="s">
+        <v>57</v>
       </c>
       <c r="B2">
         <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>987654321</v>
+      <c r="A3" s="8" t="s">
+        <v>58</v>
       </c>
       <c r="B3">
         <v>300</v>

</xml_diff>

<commit_message>
fix general intent submodules
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BrandonTan\Desktop\NLP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B463A4-0123-438D-BC35-C9F0EC0055C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A236D47D-B3F6-4B0C-9784-6E109570C998}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GENERAL_INTENTS" sheetId="2" r:id="rId1"/>
@@ -194,9 +194,6 @@
     <t>amount</t>
   </si>
   <si>
-    <t>BANK_ACC has AMOUNT left.</t>
-  </si>
-  <si>
     <t>I want to check balance in BANK_ACC.</t>
   </si>
   <si>
@@ -204,6 +201,9 @@
   </si>
   <si>
     <t>987654321</t>
+  </si>
+  <si>
+    <t>BANK_ACC bank account has AMOUNT left.</t>
   </si>
 </sst>
 </file>
@@ -511,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB0B082F-789D-46DC-A03C-2A4A6841A2A1}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -560,10 +560,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C5" s="3"/>
     </row>
@@ -828,7 +828,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE602675-32E7-41BB-B088-0029ED80F667}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -847,7 +847,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2">
         <v>200</v>
@@ -855,7 +855,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3">
         <v>300</v>

</xml_diff>

<commit_message>
updated general intent submodule in the database
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven\Documents\GitHub\NLP-bank-chatbot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BrandonTan\Desktop\NLP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0CA32CC-93C3-4ED1-A7E9-ACADE362C6F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32BE98ED-1DDB-4785-906A-F7A7DC5BCB4B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1824" yWindow="3120" windowWidth="17316" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GENERAL_INTENTS" sheetId="2" r:id="rId1"/>
@@ -98,12 +98,6 @@
     <t>Default</t>
   </si>
   <si>
-    <t>I want to transfer AMOUNT to PERSON in BANK_ACC</t>
-  </si>
-  <si>
-    <t>I want to pay bill of AMOUNT with PERSON in BANK_ACC</t>
-  </si>
-  <si>
     <t>message</t>
   </si>
   <si>
@@ -180,9 +174,6 @@
     <t>There is no expiry to your account. However, your account will be automatically deactivated if you do not login to within 6-12 months.</t>
   </si>
   <si>
-    <t>I want to deposit AMOUNT to BANK_ACC</t>
-  </si>
-  <si>
     <t>AMOUNT has been deposited into BANK_ACC.</t>
   </si>
   <si>
@@ -195,9 +186,6 @@
     <t>amount</t>
   </si>
   <si>
-    <t>I want to check balance in BANK_ACC.</t>
-  </si>
-  <si>
     <t>123456789</t>
   </si>
   <si>
@@ -217,6 +205,18 @@
   </si>
   <si>
     <t>Goodbye</t>
+  </si>
+  <si>
+    <t>I want to transfer AMOUNT to PERSON in BANK_ACC bank account.</t>
+  </si>
+  <si>
+    <t>I want to pay bill of AMOUNT with PERSON in BANK_ACC bank account</t>
+  </si>
+  <si>
+    <t>I want to deposit AMOUNT to BANK_ACC bank account</t>
+  </si>
+  <si>
+    <t>I want to check balance in BANK_ACC bank account</t>
   </si>
 </sst>
 </file>
@@ -524,59 +524,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB0B082F-789D-46DC-A03C-2A4A6841A2A1}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C5" s="3"/>
     </row>
@@ -597,21 +597,21 @@
       <selection activeCell="A18" sqref="A18:B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.140625" customWidth="1"/>
-    <col min="2" max="2" width="126.7109375" customWidth="1"/>
+    <col min="1" max="1" width="53.109375" customWidth="1"/>
+    <col min="2" max="2" width="126.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -619,7 +619,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -627,7 +627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -635,7 +635,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -643,7 +643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
@@ -651,7 +651,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -659,7 +659,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -667,7 +667,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
@@ -675,7 +675,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -683,7 +683,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -691,100 +691,100 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B13" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B16" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
+    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B17" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
+    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B18" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
+    <row r="19" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B19" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
+      <c r="B20" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="7" t="s">
+    </row>
+    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
+    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B22" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
+    <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B23" s="6" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -801,21 +801,21 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.28515625" customWidth="1"/>
-    <col min="2" max="2" width="44.140625" customWidth="1"/>
+    <col min="1" max="1" width="31.33203125" customWidth="1"/>
+    <col min="2" max="2" width="44.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
@@ -823,11 +823,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
     </row>
@@ -845,30 +845,30 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B2">
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B3">
         <v>300</v>
@@ -884,38 +884,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{200AD150-E4D5-445E-95E7-596FDC6115AF}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="105" customWidth="1"/>
-    <col min="2" max="2" width="109.7109375" customWidth="1"/>
+    <col min="2" max="2" width="109.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>